<commit_message>
Simply modified Trapezoidal Rule
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,170 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\26641\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328CF248-7368-4DEA-A66D-E8E87535D8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+  <si>
+    <t>trapezoidal_rule</t>
+  </si>
   <si>
     <t>Problem Size Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Problem size(N)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Measured Sequential Time(T1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Measured Cumulative Time</t>
   </si>
   <si>
-    <t>Measured Cumulative Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Measured Integral value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>trapezoidal_rule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>simpson_rule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Run index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Measured Sequensial Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Problem Size(Ni) ↓</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Measured MP Time(seconds) →</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Process →</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>0(10K)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1(50K)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2(100K)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3(500K)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>4(1M)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>5(5M)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>6(10M)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>7(20M)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,10 +126,183 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Consolas"/>
-      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,12 +311,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.149998474074526"/>
+        <bgColor theme="0" tint="-0.149998474074526"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -208,41 +521,327 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -250,22 +849,16 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="65" cy="172227"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="65" cy="169687"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="文本框 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A784A072-F5B2-05CE-B1F2-53B9C40E41E4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="文本框 1"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6165850" y="3092450"/>
-          <a:ext cx="65" cy="172227"/>
+          <a:off x="5785485" y="3049270"/>
+          <a:ext cx="0" cy="169545"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -302,80 +895,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57E40188-3466-49ED-8904-7622D847F352}" name="表1" displayName="表1" ref="A2:E10" totalsRowShown="0">
-  <autoFilter ref="A2:E10" xr:uid="{57E40188-3466-49ED-8904-7622D847F352}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:E10" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:E10" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3E9E7979-48C1-41E4-81BD-089D3BB784DE}" name="Problem Size Index"/>
-    <tableColumn id="2" xr3:uid="{3E19CF69-FD84-4C3E-B69A-079A677DB8CE}" name="Problem size(N)"/>
-    <tableColumn id="3" xr3:uid="{DF011E04-6231-469A-95A7-67C4DA5D05D3}" name="Measured Sequential Time(T1)"/>
-    <tableColumn id="4" xr3:uid="{548415E9-9699-4740-AAAD-42256CD3E243}" name="Measured Cumulative Time"/>
-    <tableColumn id="5" xr3:uid="{BB45452A-770E-4577-991E-A23898B7809B}" name="Measured Integral value"/>
+    <tableColumn id="1" name="Problem Size Index"/>
+    <tableColumn id="2" name="Problem size(N)"/>
+    <tableColumn id="3" name="Measured Sequential Time(T1)"/>
+    <tableColumn id="4" name="Measured Cumulative Time"/>
+    <tableColumn id="5" name="Measured Integral value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5E6B70F5-B932-4085-93FE-F7C622665FF6}" name="表1_45" displayName="表1_45" ref="A22:E30" totalsRowShown="0">
-  <autoFilter ref="A22:E30" xr:uid="{5E6B70F5-B932-4085-93FE-F7C622665FF6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_45" displayName="表1_45" ref="A22:E30" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A22:E30" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{811E2FDB-46B7-480D-9BE0-EC55C41C7E84}" name="Problem Size Index"/>
-    <tableColumn id="2" xr3:uid="{0D1E5848-E84D-484B-88F9-43CE634E82D6}" name="Problem size(N)"/>
-    <tableColumn id="3" xr3:uid="{741E347C-62FF-4814-B503-FEDAD0DA6097}" name="Measured Sequential Time(T1)"/>
-    <tableColumn id="4" xr3:uid="{2804E2E1-80A2-4994-AD68-EF55E5F72CA1}" name="Measured Cumulative Time"/>
-    <tableColumn id="5" xr3:uid="{AF07DE7F-F63E-42C0-96F5-BF3C9D487113}" name="Measured Integral value"/>
+    <tableColumn id="1" name="Problem Size Index"/>
+    <tableColumn id="2" name="Problem size(N)"/>
+    <tableColumn id="3" name="Measured Sequential Time(T1)"/>
+    <tableColumn id="4" name="Measured Cumulative Time"/>
+    <tableColumn id="5" name="Measured Integral value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{89F50B19-BC45-4363-8D1E-0CE70110AF46}" name="表6" displayName="表6" ref="A14:C19" totalsRowShown="0">
-  <autoFilter ref="A14:C19" xr:uid="{89F50B19-BC45-4363-8D1E-0CE70110AF46}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="表6" displayName="表6" ref="A14:C19" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A14:C19" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{38425375-F108-40B6-84FD-BFAB0E25585F}" name="Run index"/>
-    <tableColumn id="2" xr3:uid="{838F634C-CC07-4C55-838E-55C805DC8DC6}" name="Measured Sequensial Time"/>
-    <tableColumn id="3" xr3:uid="{E58483B7-1D7F-4651-A6CA-AC7F1AA21108}" name="Measured Cumulative Time"/>
+    <tableColumn id="1" name="Run index"/>
+    <tableColumn id="2" name="Measured Sequensial Time"/>
+    <tableColumn id="3" name="Measured Cumulative Time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{960121FB-3D64-4355-8F5C-75C66C9CE0D9}" name="表6_8" displayName="表6_8" ref="A28:C33" totalsRowShown="0">
-  <autoFilter ref="A28:C33" xr:uid="{960121FB-3D64-4355-8F5C-75C66C9CE0D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="表6_8" displayName="表6_8" ref="A28:C33" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A28:C33" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2E999EE8-4EE9-4BFC-8637-672579D7FA55}" name="Run index"/>
-    <tableColumn id="2" xr3:uid="{D2FBDBE1-7809-4A2B-B1F8-FF6ED710E432}" name="Measured Sequensial Time"/>
-    <tableColumn id="3" xr3:uid="{5C07910C-05F0-4B75-AEFB-9EFC0DCBB4F0}" name="Measured Cumulative Time"/>
+    <tableColumn id="1" name="Run index"/>
+    <tableColumn id="2" name="Measured Sequensial Time"/>
+    <tableColumn id="3" name="Measured Cumulative Time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7BCD870B-8FBC-4BE0-8261-3C0AB1BA2CDB}" name="表11" displayName="表11" ref="A3:E11" totalsRowShown="0">
-  <autoFilter ref="A3:E11" xr:uid="{7BCD870B-8FBC-4BE0-8261-3C0AB1BA2CDB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="表11" displayName="表11" ref="A3:E11" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A3:E11" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{02030258-E423-4662-A2AA-73D0C77C8B0D}" name="Process →"/>
-    <tableColumn id="2" xr3:uid="{145EF295-33A2-49AC-92FF-6159071621F6}" name="1"/>
-    <tableColumn id="3" xr3:uid="{C81B037C-2372-4E72-A494-2FE905CE4AD2}" name="2"/>
-    <tableColumn id="4" xr3:uid="{F61F69BC-BA9E-4B38-9ABE-83455E8F037A}" name="4"/>
-    <tableColumn id="5" xr3:uid="{114E355C-F78A-41B0-9EB4-5B33CE4EFC85}" name="8"/>
+    <tableColumn id="1" name="Process →"/>
+    <tableColumn id="2" name="1"/>
+    <tableColumn id="3" name="2"/>
+    <tableColumn id="4" name="4"/>
+    <tableColumn id="5" name="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{068FF9DE-1B09-4FEA-9E08-D3297ABCB652}" name="表11_13" displayName="表11_13" ref="A22:E30" totalsRowShown="0">
-  <autoFilter ref="A22:E30" xr:uid="{068FF9DE-1B09-4FEA-9E08-D3297ABCB652}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="表11_13" displayName="表11_13" ref="A22:E30" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A22:E30" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F5F460C3-C0B1-4FE8-9C29-96BADEFACB9A}" name="Process →"/>
-    <tableColumn id="2" xr3:uid="{B971746F-BF9E-48B3-BAB1-DD7CFAE58275}" name="1"/>
-    <tableColumn id="3" xr3:uid="{6878BEEA-1773-46C0-8EA2-D0FBDEEF74E9}" name="2"/>
-    <tableColumn id="4" xr3:uid="{B1484C6B-F1CB-4F31-BD9B-E7D977C124C6}" name="4"/>
-    <tableColumn id="5" xr3:uid="{0CDDE1C8-00DB-4503-9680-472255A8AEC2}" name="8"/>
+    <tableColumn id="1" name="Process →"/>
+    <tableColumn id="2" name="1"/>
+    <tableColumn id="3" name="2"/>
+    <tableColumn id="4" name="4"/>
+    <tableColumn id="5" name="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -424,7 +1017,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -459,7 +1052,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -633,71 +1226,66 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E30"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="21.4140625" customWidth="1"/>
+    <col min="1" max="1" width="21.4166666666667" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="4" width="28.08203125" customWidth="1"/>
-    <col min="5" max="5" width="24.75" customWidth="1"/>
+    <col min="3" max="4" width="28.0833333333333" customWidth="1"/>
+    <col min="5" max="5" width="33.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5">
+      <c r="A3" s="6">
         <v>0</v>
       </c>
       <c r="B3">
         <v>10000</v>
       </c>
       <c r="C3">
-        <v>1.9959999999999999E-3</v>
+        <v>0.001996</v>
       </c>
       <c r="D3">
-        <v>1.9959999999999999E-3</v>
+        <v>0.001996</v>
       </c>
       <c r="E3">
-        <v>0.19105797820000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.1910579782</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5" customHeight="1" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -705,16 +1293,16 @@
         <v>50000</v>
       </c>
       <c r="C4">
-        <v>1.2514000000000001E-2</v>
+        <v>0.012514</v>
       </c>
       <c r="D4">
-        <v>1.4511E-2</v>
+        <v>0.014511</v>
       </c>
       <c r="E4">
-        <v>0.19105771669999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910577167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2</v>
       </c>
@@ -722,16 +1310,16 @@
         <v>100000</v>
       </c>
       <c r="C5">
-        <v>4.5994E-2</v>
+        <v>0.045994</v>
       </c>
       <c r="D5">
-        <v>6.0504000000000002E-2</v>
+        <v>0.060504</v>
       </c>
       <c r="E5">
-        <v>0.19105767509999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576751</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>3</v>
       </c>
@@ -739,16 +1327,16 @@
         <v>500000</v>
       </c>
       <c r="C6">
-        <v>0.14257400000000001</v>
+        <v>0.142574</v>
       </c>
       <c r="D6">
-        <v>0.20307800000000001</v>
+        <v>0.203078</v>
       </c>
       <c r="E6">
-        <v>0.19105764040000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>4</v>
       </c>
@@ -756,16 +1344,16 @@
         <v>1000000</v>
       </c>
       <c r="C7">
-        <v>0.28497299999999998</v>
+        <v>0.284973</v>
       </c>
       <c r="D7">
-        <v>0.48805100000000001</v>
+        <v>0.488051</v>
       </c>
       <c r="E7">
-        <v>0.19105763589999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>5</v>
       </c>
@@ -779,10 +1367,10 @@
         <v>1.87639</v>
       </c>
       <c r="E8">
-        <v>0.19105763240000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>6</v>
       </c>
@@ -793,13 +1381,13 @@
         <v>2.926472</v>
       </c>
       <c r="D9">
-        <v>4.8028620000000002</v>
+        <v>4.802862</v>
       </c>
       <c r="E9">
         <v>0.1910576319</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>7</v>
       </c>
@@ -807,63 +1395,63 @@
         <v>20000000</v>
       </c>
       <c r="C10">
-        <v>5.6941309999999996</v>
+        <v>5.694131</v>
       </c>
       <c r="D10">
         <v>10.496993</v>
       </c>
       <c r="E10">
-        <v>0.19105763170000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2" t="s">
+        <v>0.1910576317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B22" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="1:5">
+      <c r="A23" s="6">
         <v>0</v>
       </c>
       <c r="B23">
         <v>10000</v>
       </c>
       <c r="C23">
-        <v>1.7520000000000001E-3</v>
+        <v>0.001752</v>
       </c>
       <c r="D23">
-        <v>1.7520000000000001E-3</v>
+        <v>0.001752</v>
       </c>
       <c r="E23">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>1</v>
       </c>
@@ -871,16 +1459,16 @@
         <v>50000</v>
       </c>
       <c r="C24">
-        <v>1.0267999999999999E-2</v>
+        <v>0.010268</v>
       </c>
       <c r="D24">
-        <v>1.2019999999999999E-2</v>
+        <v>0.01202</v>
       </c>
       <c r="E24">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>2</v>
       </c>
@@ -888,16 +1476,16 @@
         <v>100000</v>
       </c>
       <c r="C25">
-        <v>1.958E-2</v>
+        <v>0.01958</v>
       </c>
       <c r="D25">
-        <v>3.1600000000000003E-2</v>
+        <v>0.0316</v>
       </c>
       <c r="E25">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>3</v>
       </c>
@@ -905,16 +1493,16 @@
         <v>500000</v>
       </c>
       <c r="C26">
-        <v>8.4347000000000005E-2</v>
+        <v>0.084347</v>
       </c>
       <c r="D26">
-        <v>0.11594699999999999</v>
+        <v>0.115947</v>
       </c>
       <c r="E26">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>4</v>
       </c>
@@ -922,16 +1510,16 @@
         <v>1000000</v>
       </c>
       <c r="C27">
-        <v>0.17804500000000001</v>
+        <v>0.178045</v>
       </c>
       <c r="D27">
         <v>0.293993</v>
       </c>
       <c r="E27">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>5</v>
       </c>
@@ -939,16 +1527,16 @@
         <v>5000000</v>
       </c>
       <c r="C28">
-        <v>0.91752100000000003</v>
+        <v>0.917521</v>
       </c>
       <c r="D28">
         <v>1.211514</v>
       </c>
       <c r="E28">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>6</v>
       </c>
@@ -956,16 +1544,16 @@
         <v>10000000</v>
       </c>
       <c r="C29">
-        <v>1.7999700000000001</v>
+        <v>1.79997</v>
       </c>
       <c r="D29">
-        <v>3.0114830000000001</v>
+        <v>3.011483</v>
       </c>
       <c r="E29">
-        <v>0.19105763149999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1910576315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>7</v>
       </c>
@@ -973,18 +1561,18 @@
         <v>20000000</v>
       </c>
       <c r="C30">
-        <v>3.6861030000000001</v>
+        <v>3.686103</v>
       </c>
       <c r="D30">
-        <v>6.6975860000000003</v>
+        <v>6.697586</v>
       </c>
       <c r="E30">
-        <v>0.19105763149999999</v>
+        <v>0.1910576315</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
@@ -993,81 +1581,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79EC236-0429-41D3-8A3B-8CEDEE79AE16}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A13:C33"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="26.9140625" customWidth="1"/>
-    <col min="3" max="3" width="29.9140625" customWidth="1"/>
+    <col min="1" max="1" width="18.8333333333333" customWidth="1"/>
+    <col min="2" max="2" width="26.9166666666667" customWidth="1"/>
+    <col min="3" max="3" width="29.9166666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
       <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>0</v>
       </c>
       <c r="B15">
-        <v>5.8438420000000004</v>
+        <v>5.843842</v>
       </c>
       <c r="C15">
-        <v>5.8438420000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5.843842</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16">
-        <v>5.7929870000000001</v>
+        <v>5.792987</v>
       </c>
       <c r="C16">
-        <v>11.636829000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11.636829</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17">
-        <v>5.7378489999999998</v>
+        <v>5.737849</v>
       </c>
       <c r="C17">
         <v>17.374679</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18">
-        <v>5.6354639999999998</v>
+        <v>5.635464</v>
       </c>
       <c r="C18">
-        <v>23.010142999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23.010143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1075,59 +1664,59 @@
         <v>5.680434</v>
       </c>
       <c r="C19">
-        <v>28.690577000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+        <v>28.690577</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
       <c r="C28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>0</v>
       </c>
       <c r="B29">
-        <v>3.6217160000000002</v>
+        <v>3.621716</v>
       </c>
       <c r="C29">
-        <v>3.6217160000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3.621716</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>3.7123300000000001</v>
+        <v>3.71233</v>
       </c>
       <c r="C30">
-        <v>7.3340459999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7.334046</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31">
-        <v>3.6492059999999999</v>
+        <v>3.649206</v>
       </c>
       <c r="C31">
         <v>10.983252</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1138,7 +1727,7 @@
         <v>14.836062</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1146,12 +1735,12 @@
         <v>3.742019</v>
       </c>
       <c r="C33">
-        <v>18.578081000000001</v>
+        <v>18.578081</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
@@ -1160,75 +1749,76 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985382A2-2CA9-45CB-8C4C-39BFAF920068}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.83333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>9.554E-2</v>
+        <v>0.09554</v>
       </c>
       <c r="C4">
-        <v>7.8103000000000006E-2</v>
+        <v>0.078103</v>
       </c>
       <c r="D4">
         <v>0.114581</v>
       </c>
       <c r="E4">
-        <v>0.12520600000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.125206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>7.9532000000000005E-2</v>
+        <v>0.079532</v>
       </c>
       <c r="C5">
-        <v>9.0612999999999999E-2</v>
+        <v>0.090613</v>
       </c>
       <c r="D5">
         <v>0.104167</v>
@@ -1237,9 +1827,9 @@
         <v>0.125692</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0.103811</v>
@@ -1254,192 +1844,192 @@
         <v>0.134044</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7">
-        <v>0.19755700000000001</v>
+        <v>0.197557</v>
       </c>
       <c r="C7">
-        <v>0.17754400000000001</v>
+        <v>0.177544</v>
       </c>
       <c r="D7">
-        <v>0.17089499999999999</v>
+        <v>0.170895</v>
       </c>
       <c r="E7">
         <v>0.185782</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>0.35599999999999998</v>
+        <v>0.356</v>
       </c>
       <c r="C8">
-        <v>0.25028499999999998</v>
+        <v>0.250285</v>
       </c>
       <c r="D8">
         <v>0.217915</v>
       </c>
       <c r="E8">
-        <v>0.20949999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.2095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>1.456318</v>
       </c>
       <c r="C9">
-        <v>0.84288300000000005</v>
+        <v>0.842883</v>
       </c>
       <c r="D9">
-        <v>0.55520700000000001</v>
+        <v>0.555207</v>
       </c>
       <c r="E9">
-        <v>0.46351999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.46352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>2.7560220000000002</v>
+        <v>2.756022</v>
       </c>
       <c r="C10">
-        <v>1.6147670000000001</v>
+        <v>1.614767</v>
       </c>
       <c r="D10">
         <v>1.012732</v>
       </c>
       <c r="E10">
-        <v>0.78809899999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.788099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>5.5579859999999996</v>
+        <v>5.557986</v>
       </c>
       <c r="C11">
-        <v>3.2290649999999999</v>
+        <v>3.229065</v>
       </c>
       <c r="D11">
         <v>1.964234</v>
       </c>
       <c r="E11">
-        <v>1.3654459999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+        <v>1.365446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="4" t="s">
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B23">
         <v>0.108261</v>
       </c>
       <c r="C23">
-        <v>8.4815000000000002E-2</v>
+        <v>0.084815</v>
       </c>
       <c r="D23">
-        <v>9.7840999999999997E-2</v>
+        <v>0.097841</v>
       </c>
       <c r="E23">
         <v>0.105881</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>7.9565999999999998E-2</v>
+        <v>0.079566</v>
       </c>
       <c r="C24">
-        <v>8.7429999999999994E-2</v>
+        <v>0.08743</v>
       </c>
       <c r="D24">
         <v>0.10425</v>
       </c>
       <c r="E24">
-        <v>0.12604000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.12604</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B25">
-        <v>8.4720000000000004E-2</v>
+        <v>0.08472</v>
       </c>
       <c r="C25">
-        <v>0.10174999999999999</v>
+        <v>0.10175</v>
       </c>
       <c r="D25">
-        <v>0.11050500000000001</v>
+        <v>0.110505</v>
       </c>
       <c r="E25">
-        <v>0.13004399999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.130044</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B26">
-        <v>0.16073599999999999</v>
+        <v>0.160736</v>
       </c>
       <c r="C26">
         <v>0.146368</v>
       </c>
       <c r="D26">
-        <v>0.15142900000000001</v>
+        <v>0.151429</v>
       </c>
       <c r="E26">
-        <v>0.16181400000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.161814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B27">
         <v>0.42879</v>
@@ -1448,52 +2038,52 @@
         <v>0.199404</v>
       </c>
       <c r="D27">
-        <v>0.17770900000000001</v>
+        <v>0.177709</v>
       </c>
       <c r="E27">
         <v>0.195771</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B28">
-        <v>1.0019450000000001</v>
+        <v>1.001945</v>
       </c>
       <c r="C28">
-        <v>0.58983099999999999</v>
+        <v>0.589831</v>
       </c>
       <c r="D28">
-        <v>0.39045099999999999</v>
+        <v>0.390451</v>
       </c>
       <c r="E28">
-        <v>0.35623700000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.356237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B29">
         <v>1.862168</v>
       </c>
       <c r="C29">
-        <v>1.1919690000000001</v>
+        <v>1.191969</v>
       </c>
       <c r="D29">
-        <v>0.69228500000000004</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0.54488099999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.692285</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.544881</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B30">
-        <v>3.6356670000000002</v>
+        <v>3.635667</v>
       </c>
       <c r="C30">
         <v>2.033833</v>
@@ -1502,15 +2092,15 @@
         <v>1.275701</v>
       </c>
       <c r="E30">
-        <v>0.92589699999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+        <v>0.925897</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>